<commit_message>
Code cleanup before adding command structure
</commit_message>
<xml_diff>
--- a/documentation/Command Mapping.xlsx
+++ b/documentation/Command Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\Development\GitHub\Vantage-Pro2-Console\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539019F1-7B80-49DB-9C9B-44EE5E747839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39C6FB7-EEC0-40CB-A84E-04842AAC151A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3A335B6C-A0AB-4193-B99C-C41C0FF65E63}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="100">
   <si>
     <t>TEST</t>
   </si>
@@ -330,13 +330,40 @@
   </si>
   <si>
     <t>backlight</t>
+  </si>
+  <si>
+    <t>console-diagnostics</t>
+  </si>
+  <si>
+    <r>
+      <t>console-recovery-clear-</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>crc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>-error-count</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +385,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -713,7 +753,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +761,7 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -776,6 +816,9 @@
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -786,6 +829,9 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed unused command names and updated command mapping spreadsheet
</commit_message>
<xml_diff>
--- a/documentation/Command Mapping.xlsx
+++ b/documentation/Command Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\Development\GitHub\Vantage-Pro2-Console\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39C6FB7-EEC0-40CB-A84E-04842AAC151A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7F4525-0B96-4DC9-B039-ABCC08EDE77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3A335B6C-A0AB-4193-B99C-C41C0FF65E63}"/>
+    <workbookView xWindow="-23138" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{3A335B6C-A0AB-4193-B99C-C41C0FF65E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="114">
   <si>
     <t>TEST</t>
   </si>
@@ -321,12 +321,6 @@
   </si>
   <si>
     <t>firmware-query</t>
-  </si>
-  <si>
-    <t>set-date-time</t>
-  </si>
-  <si>
-    <t>get-date-time</t>
   </si>
   <si>
     <t>backlight</t>
@@ -357,6 +351,54 @@
       </rPr>
       <t>-error-count</t>
     </r>
+  </si>
+  <si>
+    <t>clear-alarm-thresholds</t>
+  </si>
+  <si>
+    <t>clear-console-archive</t>
+  </si>
+  <si>
+    <t>clear-calibration-offsets</t>
+  </si>
+  <si>
+    <t>clear-graph-points</t>
+  </si>
+  <si>
+    <t>clear-active-alarms</t>
+  </si>
+  <si>
+    <t>clear-current-data</t>
+  </si>
+  <si>
+    <t>query-console-time</t>
+  </si>
+  <si>
+    <t>update-archive-period</t>
+  </si>
+  <si>
+    <t>stop-archiving</t>
+  </si>
+  <si>
+    <t>start-archiving</t>
+  </si>
+  <si>
+    <t>put-year-rain</t>
+  </si>
+  <si>
+    <t>put-year-et</t>
+  </si>
+  <si>
+    <t>clear-cumulative-values</t>
+  </si>
+  <si>
+    <t>clear-high-values, clear-highs</t>
+  </si>
+  <si>
+    <t>clear-low-values, clear-lows</t>
+  </si>
+  <si>
+    <t>query-hilows</t>
   </si>
 </sst>
 </file>
@@ -753,7 +795,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +859,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -831,7 +873,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,6 +953,9 @@
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -922,6 +967,9 @@
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -933,6 +981,9 @@
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D13" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -973,7 +1024,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -984,7 +1035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -995,7 +1046,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1006,7 +1057,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -1017,7 +1068,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -1028,7 +1079,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -1039,7 +1090,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1050,7 +1101,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -1061,7 +1112,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -1071,8 +1122,11 @@
       <c r="C25" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -1082,8 +1136,11 @@
       <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -1093,8 +1150,11 @@
       <c r="C27" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -1104,8 +1164,11 @@
       <c r="C28" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -1115,8 +1178,11 @@
       <c r="C29" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>90</v>
       </c>
@@ -1126,8 +1192,11 @@
       <c r="C30" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -1137,8 +1206,11 @@
       <c r="C31" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -1147,6 +1219,9 @@
       </c>
       <c r="C32" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="D32" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1159,6 +1234,9 @@
       <c r="C33" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="D33" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1185,7 +1263,7 @@
         <v>67</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1213,7 +1291,7 @@
         <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1226,6 +1304,9 @@
       <c r="C38" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="D38" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1237,6 +1318,9 @@
       <c r="C39" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1248,6 +1332,9 @@
       <c r="C40" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="D40" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1274,7 +1361,7 @@
         <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>